<commit_message>
Sped up logbook code, added more data
</commit_message>
<xml_diff>
--- a/Logbook_automated_by_python_testing.xlsx
+++ b/Logbook_automated_by_python_testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e67038fc02b579b/Documenten/GitHub/tidegas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_0319ED24126AC40F62355476585DCE3A87459430" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_48E939DDD451CE0F62355476585DCE3A87446097" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{372AD253-00D3-480E-9175-FAA81A7AC985}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="218">
   <si>
     <t>Description</t>
   </si>
@@ -569,6 +569,111 @@
   </si>
   <si>
     <t>0-0  0  (0)nose-251017-04-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251021-01-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>21-Oct</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-01-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>22-Oct</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-02-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-03-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-04-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-05-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-06-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-07-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-08-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-09-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-10-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-11-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-12-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-13-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-14-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251022-15-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)junk-251023-01-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>23-Oct</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-02-4_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-03-3_6mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-04-3_0mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-05-2_4mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-06-2_1mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-07-1_8mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-08-1_5mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-09-1_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-10-1_2mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-11-0_6mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-12-0_15mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-13-0_0mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-14-0_15mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-15-0_15mL-0_15incrmL.dat</t>
+  </si>
+  <si>
+    <t>0-0  0  (0)nose-251023-16-0_0mL-0_15incrmL.dat</t>
   </si>
 </sst>
 </file>
@@ -931,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF130"/>
+  <dimension ref="A1:AF162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="P126" sqref="P126"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159:F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1739,7 +1844,7 @@
         <v>2379.7790873880422</v>
       </c>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>54</v>
       </c>
@@ -1786,7 +1891,7 @@
         <v>2380.427060397808</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>55</v>
       </c>
@@ -1833,7 +1938,7 @@
         <v>2383.1221525679371</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>56</v>
       </c>
@@ -1880,7 +1985,7 @@
         <v>2382.290757545321</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>57</v>
       </c>
@@ -1927,7 +2032,7 @@
         <v>2382.0903488719409</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>58</v>
       </c>
@@ -1974,7 +2079,7 @@
         <v>2385.7030338880641</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>59</v>
       </c>
@@ -2024,7 +2129,7 @@
         <v>2381.3069655385671</v>
       </c>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>60</v>
       </c>
@@ -2055,9 +2160,6 @@
       <c r="O23">
         <v>2255.986084078414</v>
       </c>
-      <c r="Q23">
-        <v>2068.891307858692</v>
-      </c>
       <c r="V23">
         <v>4.2</v>
       </c>
@@ -2074,7 +2176,7 @@
         <v>2380.499045287635</v>
       </c>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>61</v>
       </c>
@@ -2121,7 +2223,7 @@
         <v>2383.0631379730412</v>
       </c>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>62</v>
       </c>
@@ -2152,6 +2254,9 @@
       <c r="O25">
         <v>2255.986084078414</v>
       </c>
+      <c r="V25">
+        <v>4.2</v>
+      </c>
       <c r="W25">
         <v>0.15</v>
       </c>
@@ -2165,7 +2270,7 @@
         <v>2365.5849331188451</v>
       </c>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>64</v>
       </c>
@@ -2196,6 +2301,9 @@
       <c r="O26">
         <v>2255.986084078414</v>
       </c>
+      <c r="V26">
+        <v>4.2</v>
+      </c>
       <c r="W26">
         <v>0.15</v>
       </c>
@@ -2209,7 +2317,7 @@
         <v>2335.973572859863</v>
       </c>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>65</v>
       </c>
@@ -2240,6 +2348,9 @@
       <c r="O27">
         <v>2255.986084078414</v>
       </c>
+      <c r="V27">
+        <v>4.2</v>
+      </c>
       <c r="W27">
         <v>0.15</v>
       </c>
@@ -2253,7 +2364,7 @@
         <v>2351.1448877322518</v>
       </c>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>66</v>
       </c>
@@ -2300,7 +2411,7 @@
         <v>2353.526902313195</v>
       </c>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>68</v>
       </c>
@@ -2313,6 +2424,9 @@
       <c r="E29">
         <v>3</v>
       </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
       <c r="J29">
         <v>25</v>
       </c>
@@ -2331,6 +2445,12 @@
       <c r="O29">
         <v>2274.242388753104</v>
       </c>
+      <c r="P29">
+        <v>1650.4814576741401</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
       <c r="V29">
         <v>4.2</v>
       </c>
@@ -2346,8 +2466,11 @@
       <c r="AA29">
         <v>2346.5180077152991</v>
       </c>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AF29">
+        <v>1682.7805000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -2360,6 +2483,9 @@
       <c r="E30">
         <v>4</v>
       </c>
+      <c r="G30">
+        <v>15</v>
+      </c>
       <c r="J30">
         <v>25</v>
       </c>
@@ -2378,14 +2504,23 @@
       <c r="O30">
         <v>2274.242388753104</v>
       </c>
+      <c r="P30">
+        <v>1867.2677651954241</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
       <c r="V30">
         <v>2.25</v>
       </c>
       <c r="W30">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AF30">
+        <v>1903.8091999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>70</v>
       </c>
@@ -2398,6 +2533,9 @@
       <c r="E31">
         <v>5</v>
       </c>
+      <c r="G31">
+        <v>16</v>
+      </c>
       <c r="J31">
         <v>25</v>
       </c>
@@ -2416,6 +2554,12 @@
       <c r="O31">
         <v>2274.242388753104</v>
       </c>
+      <c r="P31">
+        <v>2086.960593651359</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
       <c r="V31">
         <v>1.2</v>
       </c>
@@ -2431,8 +2575,11 @@
       <c r="AA31">
         <v>293.50828195330507</v>
       </c>
-    </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AF31">
+        <v>2127.8013000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>71</v>
       </c>
@@ -2445,6 +2592,9 @@
       <c r="E32">
         <v>6</v>
       </c>
+      <c r="G32">
+        <v>17</v>
+      </c>
       <c r="J32">
         <v>25.1</v>
       </c>
@@ -2463,6 +2613,12 @@
       <c r="O32">
         <v>2274.308809236642</v>
       </c>
+      <c r="P32">
+        <v>1768.674938691129</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
       <c r="V32">
         <v>3.15</v>
       </c>
@@ -2477,6 +2633,9 @@
       </c>
       <c r="AA32">
         <v>2354.516151707568</v>
+      </c>
+      <c r="AF32">
+        <v>1803.2343000000001</v>
       </c>
     </row>
     <row r="33" spans="2:32" x14ac:dyDescent="0.3">
@@ -2492,6 +2651,9 @@
       <c r="E33">
         <v>7</v>
       </c>
+      <c r="G33">
+        <v>18</v>
+      </c>
       <c r="J33">
         <v>25.2</v>
       </c>
@@ -2510,6 +2672,12 @@
       <c r="O33">
         <v>2274.375411340548</v>
       </c>
+      <c r="P33">
+        <v>1684.514500298744</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
       <c r="V33">
         <v>3.6</v>
       </c>
@@ -2524,6 +2692,9 @@
       </c>
       <c r="AA33">
         <v>2350.0741610478558</v>
+      </c>
+      <c r="AF33">
+        <v>1717.3791000000001</v>
       </c>
     </row>
     <row r="34" spans="2:32" x14ac:dyDescent="0.3">
@@ -2539,6 +2710,9 @@
       <c r="E34">
         <v>8</v>
       </c>
+      <c r="G34">
+        <v>21</v>
+      </c>
       <c r="J34">
         <v>25.2</v>
       </c>
@@ -2557,6 +2731,12 @@
       <c r="O34">
         <v>2274.375411340548</v>
       </c>
+      <c r="P34">
+        <v>1566.6935672443669</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
       <c r="V34">
         <v>4.8</v>
       </c>
@@ -2571,6 +2751,9 @@
       </c>
       <c r="AA34">
         <v>2354.9775513610289</v>
+      </c>
+      <c r="AF34">
+        <v>1597.2594999999999</v>
       </c>
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.3">
@@ -2633,6 +2816,9 @@
       <c r="E36">
         <v>1</v>
       </c>
+      <c r="G36">
+        <v>24</v>
+      </c>
       <c r="J36">
         <v>24.7</v>
       </c>
@@ -2651,18 +2837,18 @@
       <c r="O36">
         <v>2247.2038067669282</v>
       </c>
+      <c r="P36">
+        <v>1626.0041952186909</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
       <c r="R36">
         <v>821</v>
       </c>
       <c r="S36" t="s">
         <v>77</v>
       </c>
-      <c r="T36">
-        <v>4.2</v>
-      </c>
-      <c r="U36">
-        <v>0.15</v>
-      </c>
       <c r="V36">
         <v>4.2</v>
       </c>
@@ -2677,6 +2863,9 @@
       </c>
       <c r="AA36">
         <v>2353.8406690606562</v>
+      </c>
+      <c r="AF36">
+        <v>1657.9686999999999</v>
       </c>
     </row>
     <row r="37" spans="2:32" x14ac:dyDescent="0.3">
@@ -2692,6 +2881,9 @@
       <c r="E37">
         <v>2</v>
       </c>
+      <c r="G37">
+        <v>25</v>
+      </c>
       <c r="J37">
         <v>25</v>
       </c>
@@ -2710,18 +2902,18 @@
       <c r="O37">
         <v>2247.3996370943469</v>
       </c>
+      <c r="P37">
+        <v>1887.7676925448279</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
       <c r="R37">
         <v>555</v>
       </c>
       <c r="S37" t="s">
         <v>77</v>
       </c>
-      <c r="T37">
-        <v>2.25</v>
-      </c>
-      <c r="U37">
-        <v>0.15</v>
-      </c>
       <c r="V37">
         <v>2.25</v>
       </c>
@@ -2736,6 +2928,9 @@
       </c>
       <c r="AA37">
         <v>1473.9676953059411</v>
+      </c>
+      <c r="AF37">
+        <v>1924.7103</v>
       </c>
     </row>
     <row r="38" spans="2:32" x14ac:dyDescent="0.3">
@@ -2751,6 +2946,9 @@
       <c r="E38">
         <v>3</v>
       </c>
+      <c r="G38">
+        <v>26</v>
+      </c>
       <c r="J38">
         <v>25</v>
       </c>
@@ -2769,11 +2967,11 @@
       <c r="O38">
         <v>2247.3996370943469</v>
       </c>
-      <c r="T38">
-        <v>1.2</v>
-      </c>
-      <c r="U38">
-        <v>0.15</v>
+      <c r="P38">
+        <v>2073.6655701738082</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
       </c>
       <c r="V38">
         <v>1.2</v>
@@ -2789,6 +2987,9 @@
       </c>
       <c r="AA38">
         <v>316.44527370375539</v>
+      </c>
+      <c r="AF38">
+        <v>2114.2460999999998</v>
       </c>
     </row>
     <row r="39" spans="2:32" x14ac:dyDescent="0.3">
@@ -2804,6 +3005,9 @@
       <c r="E39">
         <v>4</v>
       </c>
+      <c r="G39">
+        <v>27</v>
+      </c>
       <c r="J39">
         <v>25.2</v>
       </c>
@@ -2822,11 +3026,11 @@
       <c r="O39">
         <v>2247.5310896238698</v>
       </c>
-      <c r="T39">
-        <v>1.2</v>
-      </c>
-      <c r="U39">
-        <v>0.15</v>
+      <c r="P39">
+        <v>2022.103396683485</v>
+      </c>
+      <c r="Q39">
+        <v>0.5</v>
       </c>
       <c r="V39">
         <v>1.2</v>
@@ -2842,6 +3046,9 @@
       </c>
       <c r="AA39">
         <v>321.92057616761798</v>
+      </c>
+      <c r="AF39">
+        <v>2061.5542999999998</v>
       </c>
     </row>
     <row r="40" spans="2:32" x14ac:dyDescent="0.3">
@@ -2857,6 +3064,9 @@
       <c r="E40">
         <v>5</v>
       </c>
+      <c r="G40">
+        <v>28</v>
+      </c>
       <c r="J40">
         <v>25.2</v>
       </c>
@@ -2875,11 +3085,11 @@
       <c r="O40">
         <v>2247.5310896238698</v>
       </c>
-      <c r="T40">
-        <v>1.2</v>
-      </c>
-      <c r="U40">
-        <v>0.15</v>
+      <c r="P40">
+        <v>2071.4397525288991</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
       </c>
       <c r="V40">
         <v>1.2</v>
@@ -2895,6 +3105,9 @@
       </c>
       <c r="AA40">
         <v>322.35424204536741</v>
+      </c>
+      <c r="AF40">
+        <v>2111.8532</v>
       </c>
     </row>
     <row r="41" spans="2:32" x14ac:dyDescent="0.3">
@@ -2910,6 +3123,9 @@
       <c r="E41">
         <v>7</v>
       </c>
+      <c r="G41">
+        <v>29</v>
+      </c>
       <c r="J41">
         <v>25.2</v>
       </c>
@@ -2928,18 +3144,18 @@
       <c r="O41">
         <v>2247.5310896238698</v>
       </c>
+      <c r="P41">
+        <v>1906.5536530976669</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
       <c r="R41">
         <v>539</v>
       </c>
       <c r="S41" t="s">
         <v>77</v>
       </c>
-      <c r="T41">
-        <v>2.25</v>
-      </c>
-      <c r="U41">
-        <v>0.15</v>
-      </c>
       <c r="V41">
         <v>2.25</v>
       </c>
@@ -2954,6 +3170,9 @@
       </c>
       <c r="AA41">
         <v>1381.7065763197461</v>
+      </c>
+      <c r="AF41">
+        <v>1943.7501999999999</v>
       </c>
     </row>
     <row r="42" spans="2:32" x14ac:dyDescent="0.3">
@@ -2969,6 +3188,9 @@
       <c r="E42">
         <v>8</v>
       </c>
+      <c r="G42">
+        <v>30</v>
+      </c>
       <c r="J42">
         <v>25.21</v>
       </c>
@@ -2987,18 +3209,18 @@
       <c r="O42">
         <v>2247.5376810862308</v>
       </c>
+      <c r="P42">
+        <v>1897.699863135228</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
       <c r="R42">
         <v>548</v>
       </c>
       <c r="S42" t="s">
         <v>77</v>
       </c>
-      <c r="T42">
-        <v>2.25</v>
-      </c>
-      <c r="U42">
-        <v>0.15</v>
-      </c>
       <c r="V42">
         <v>2.25</v>
       </c>
@@ -3013,6 +3235,9 @@
       </c>
       <c r="AA42">
         <v>1379.0636853083431</v>
+      </c>
+      <c r="AF42">
+        <v>1934.7180000000001</v>
       </c>
     </row>
     <row r="43" spans="2:32" x14ac:dyDescent="0.3">
@@ -3028,6 +3253,9 @@
       <c r="E43">
         <v>9</v>
       </c>
+      <c r="G43">
+        <v>31</v>
+      </c>
       <c r="J43">
         <v>25</v>
       </c>
@@ -3046,18 +3274,18 @@
       <c r="O43">
         <v>2247.3996370943469</v>
       </c>
+      <c r="P43">
+        <v>1892.8755347947681</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
       <c r="R43">
         <v>561</v>
       </c>
       <c r="S43" t="s">
         <v>77</v>
       </c>
-      <c r="T43">
-        <v>2.25</v>
-      </c>
-      <c r="U43">
-        <v>0.15</v>
-      </c>
       <c r="V43">
         <v>2.25</v>
       </c>
@@ -3072,6 +3300,9 @@
       </c>
       <c r="AA43">
         <v>1376.2698085921641</v>
+      </c>
+      <c r="AF43">
+        <v>1929.9181000000001</v>
       </c>
     </row>
     <row r="44" spans="2:32" x14ac:dyDescent="0.3">
@@ -3087,6 +3318,9 @@
       <c r="E44">
         <v>10</v>
       </c>
+      <c r="G44">
+        <v>32</v>
+      </c>
       <c r="J44">
         <v>25</v>
       </c>
@@ -3105,15 +3339,15 @@
       <c r="O44">
         <v>2247.3996370943469</v>
       </c>
+      <c r="P44">
+        <v>1761.999410777345</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
       <c r="R44">
         <v>697</v>
       </c>
-      <c r="T44">
-        <v>3.15</v>
-      </c>
-      <c r="U44">
-        <v>0.15</v>
-      </c>
       <c r="V44">
         <v>3.15</v>
       </c>
@@ -3128,6 +3362,9 @@
       </c>
       <c r="AA44">
         <v>2372.2945507453628</v>
+      </c>
+      <c r="AF44">
+        <v>1796.4808</v>
       </c>
     </row>
     <row r="45" spans="2:32" x14ac:dyDescent="0.3">
@@ -3143,6 +3380,9 @@
       <c r="E45">
         <v>11</v>
       </c>
+      <c r="G45">
+        <v>33</v>
+      </c>
       <c r="J45">
         <v>25.1</v>
       </c>
@@ -3161,15 +3401,15 @@
       <c r="O45">
         <v>2247.4652736207522</v>
       </c>
+      <c r="P45">
+        <v>1776.503863913513</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
       <c r="R45">
         <v>690</v>
       </c>
-      <c r="T45">
-        <v>3.15</v>
-      </c>
-      <c r="U45">
-        <v>0.15</v>
-      </c>
       <c r="V45">
         <v>3.15</v>
       </c>
@@ -3184,6 +3424,9 @@
       </c>
       <c r="AA45">
         <v>2371.0065608492009</v>
+      </c>
+      <c r="AF45">
+        <v>1811.2162000000001</v>
       </c>
     </row>
     <row r="46" spans="2:32" x14ac:dyDescent="0.3">
@@ -3199,6 +3442,9 @@
       <c r="E46">
         <v>12</v>
       </c>
+      <c r="G46">
+        <v>34</v>
+      </c>
       <c r="J46">
         <v>24.8</v>
       </c>
@@ -3217,15 +3463,15 @@
       <c r="O46">
         <v>2247.2689034275022</v>
       </c>
+      <c r="P46">
+        <v>1655.9529638285719</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
       <c r="R46">
         <v>803</v>
       </c>
-      <c r="T46">
-        <v>4.2</v>
-      </c>
-      <c r="U46">
-        <v>0.15</v>
-      </c>
       <c r="V46">
         <v>4.2</v>
       </c>
@@ -3240,6 +3486,9 @@
       </c>
       <c r="AA46">
         <v>2370.6613934554248</v>
+      </c>
+      <c r="AF46">
+        <v>1688.4573</v>
       </c>
     </row>
     <row r="47" spans="2:32" x14ac:dyDescent="0.3">
@@ -3255,6 +3504,9 @@
       <c r="E47">
         <v>13</v>
       </c>
+      <c r="G47">
+        <v>35</v>
+      </c>
       <c r="J47">
         <v>25</v>
       </c>
@@ -3273,11 +3525,11 @@
       <c r="O47">
         <v>2247.3996370943469</v>
       </c>
-      <c r="T47">
-        <v>4.2</v>
-      </c>
-      <c r="U47">
-        <v>0.15</v>
+      <c r="P47">
+        <v>1668.6995395236229</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
       </c>
       <c r="V47">
         <v>4.2</v>
@@ -3293,6 +3545,9 @@
       </c>
       <c r="AA47">
         <v>2372.7084622496941</v>
+      </c>
+      <c r="AF47">
+        <v>1701.3551</v>
       </c>
     </row>
     <row r="48" spans="2:32" x14ac:dyDescent="0.3">
@@ -7815,6 +8070,1789 @@
       </c>
       <c r="AF130">
         <v>1755.0399</v>
+      </c>
+    </row>
+    <row r="131" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>183</v>
+      </c>
+      <c r="C131" t="s">
+        <v>184</v>
+      </c>
+      <c r="D131" t="s">
+        <v>147</v>
+      </c>
+      <c r="E131">
+        <v>1</v>
+      </c>
+      <c r="J131">
+        <v>25</v>
+      </c>
+      <c r="K131">
+        <v>178.65</v>
+      </c>
+      <c r="L131">
+        <v>30</v>
+      </c>
+      <c r="M131">
+        <v>0.1</v>
+      </c>
+      <c r="V131">
+        <v>4.2</v>
+      </c>
+      <c r="W131">
+        <v>0.15</v>
+      </c>
+      <c r="X131">
+        <v>633.32404256933614</v>
+      </c>
+      <c r="Z131">
+        <v>2222.4181336354291</v>
+      </c>
+    </row>
+    <row r="132" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>185</v>
+      </c>
+      <c r="C132" t="s">
+        <v>186</v>
+      </c>
+      <c r="D132" t="s">
+        <v>147</v>
+      </c>
+      <c r="E132">
+        <v>1</v>
+      </c>
+      <c r="G132">
+        <v>179</v>
+      </c>
+      <c r="J132">
+        <v>24.9</v>
+      </c>
+      <c r="K132">
+        <v>175.95</v>
+      </c>
+      <c r="L132">
+        <v>30</v>
+      </c>
+      <c r="M132">
+        <v>0.1</v>
+      </c>
+      <c r="N132">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O132">
+        <v>2263.5673144353809</v>
+      </c>
+      <c r="P132">
+        <v>1672.276480089083</v>
+      </c>
+      <c r="Q132">
+        <v>0</v>
+      </c>
+      <c r="V132">
+        <v>4.2</v>
+      </c>
+      <c r="W132">
+        <v>0.15</v>
+      </c>
+      <c r="X132">
+        <v>633.21787308521368</v>
+      </c>
+      <c r="Z132">
+        <v>2285.7394999962571</v>
+      </c>
+      <c r="AF132">
+        <v>1705.0517</v>
+      </c>
+    </row>
+    <row r="133" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>187</v>
+      </c>
+      <c r="C133" t="s">
+        <v>186</v>
+      </c>
+      <c r="D133" t="s">
+        <v>147</v>
+      </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+      <c r="G133">
+        <v>180</v>
+      </c>
+      <c r="J133">
+        <v>25.1</v>
+      </c>
+      <c r="K133">
+        <v>176.3</v>
+      </c>
+      <c r="L133">
+        <v>30</v>
+      </c>
+      <c r="M133">
+        <v>0.1</v>
+      </c>
+      <c r="N133">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O133">
+        <v>2263.699354697188</v>
+      </c>
+      <c r="P133">
+        <v>1961.925875158729</v>
+      </c>
+      <c r="Q133">
+        <v>0</v>
+      </c>
+      <c r="V133">
+        <v>2.1</v>
+      </c>
+      <c r="W133">
+        <v>0.15</v>
+      </c>
+      <c r="X133">
+        <v>504.45439009690591</v>
+      </c>
+      <c r="Z133">
+        <v>1073.982738855552</v>
+      </c>
+      <c r="AF133">
+        <v>2000.2612999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>188</v>
+      </c>
+      <c r="C134" t="s">
+        <v>186</v>
+      </c>
+      <c r="D134" t="s">
+        <v>147</v>
+      </c>
+      <c r="E134">
+        <v>3</v>
+      </c>
+      <c r="G134">
+        <v>181</v>
+      </c>
+      <c r="J134">
+        <v>25.1</v>
+      </c>
+      <c r="K134">
+        <v>176.5</v>
+      </c>
+      <c r="L134">
+        <v>30</v>
+      </c>
+      <c r="M134">
+        <v>0.1</v>
+      </c>
+      <c r="N134">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O134">
+        <v>2263.699354697188</v>
+      </c>
+      <c r="P134">
+        <v>1976.8547691864439</v>
+      </c>
+      <c r="Q134">
+        <v>0</v>
+      </c>
+      <c r="V134">
+        <v>2.1</v>
+      </c>
+      <c r="W134">
+        <v>0.15</v>
+      </c>
+      <c r="X134">
+        <v>503.94041125568037</v>
+      </c>
+      <c r="Z134">
+        <v>1070.706084467477</v>
+      </c>
+      <c r="AF134">
+        <v>2015.4819</v>
+      </c>
+    </row>
+    <row r="135" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>189</v>
+      </c>
+      <c r="C135" t="s">
+        <v>186</v>
+      </c>
+      <c r="D135" t="s">
+        <v>147</v>
+      </c>
+      <c r="E135">
+        <v>4</v>
+      </c>
+      <c r="G135">
+        <v>182</v>
+      </c>
+      <c r="J135">
+        <v>25.1</v>
+      </c>
+      <c r="K135">
+        <v>176.6</v>
+      </c>
+      <c r="L135">
+        <v>30</v>
+      </c>
+      <c r="M135">
+        <v>0.1</v>
+      </c>
+      <c r="N135">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O135">
+        <v>2263.699354697188</v>
+      </c>
+      <c r="P135">
+        <v>1923.9591335479349</v>
+      </c>
+      <c r="Q135">
+        <v>1</v>
+      </c>
+      <c r="V135">
+        <v>2.1</v>
+      </c>
+      <c r="W135">
+        <v>0.15</v>
+      </c>
+      <c r="X135">
+        <v>500.7942265723575</v>
+      </c>
+      <c r="Z135">
+        <v>986.11553317651192</v>
+      </c>
+      <c r="AF135">
+        <v>1961.5527</v>
+      </c>
+    </row>
+    <row r="136" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>190</v>
+      </c>
+      <c r="C136" t="s">
+        <v>186</v>
+      </c>
+      <c r="D136" t="s">
+        <v>147</v>
+      </c>
+      <c r="E136">
+        <v>5</v>
+      </c>
+      <c r="G136">
+        <v>183</v>
+      </c>
+      <c r="J136">
+        <v>25.2</v>
+      </c>
+      <c r="K136">
+        <v>177.2</v>
+      </c>
+      <c r="L136">
+        <v>30</v>
+      </c>
+      <c r="M136">
+        <v>0.1</v>
+      </c>
+      <c r="N136">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O136">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="P136">
+        <v>1933.0683556301919</v>
+      </c>
+      <c r="Q136">
+        <v>1</v>
+      </c>
+      <c r="V136">
+        <v>2.1</v>
+      </c>
+      <c r="W136">
+        <v>0.15</v>
+      </c>
+      <c r="X136">
+        <v>500.80730341006921</v>
+      </c>
+      <c r="Z136">
+        <v>985.99723635226871</v>
+      </c>
+      <c r="AF136">
+        <v>1970.7822000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>191</v>
+      </c>
+      <c r="C137" t="s">
+        <v>186</v>
+      </c>
+      <c r="D137" t="s">
+        <v>147</v>
+      </c>
+      <c r="E137">
+        <v>6</v>
+      </c>
+      <c r="G137">
+        <v>185</v>
+      </c>
+      <c r="J137">
+        <v>25.1</v>
+      </c>
+      <c r="K137">
+        <v>176.95</v>
+      </c>
+      <c r="L137">
+        <v>30</v>
+      </c>
+      <c r="M137">
+        <v>0.1</v>
+      </c>
+      <c r="N137">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O137">
+        <v>2263.699354697188</v>
+      </c>
+      <c r="P137">
+        <v>1890.943645964704</v>
+      </c>
+      <c r="Q137">
+        <v>2</v>
+      </c>
+      <c r="V137">
+        <v>2.1</v>
+      </c>
+      <c r="W137">
+        <v>0.15</v>
+      </c>
+      <c r="X137">
+        <v>500.71956891049069</v>
+      </c>
+      <c r="Z137">
+        <v>985.04539221408947</v>
+      </c>
+      <c r="AF137">
+        <v>1927.8921</v>
+      </c>
+    </row>
+    <row r="138" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>192</v>
+      </c>
+      <c r="C138" t="s">
+        <v>186</v>
+      </c>
+      <c r="D138" t="s">
+        <v>147</v>
+      </c>
+      <c r="E138">
+        <v>7</v>
+      </c>
+      <c r="G138">
+        <v>186</v>
+      </c>
+      <c r="J138">
+        <v>25.2</v>
+      </c>
+      <c r="K138">
+        <v>177.15</v>
+      </c>
+      <c r="L138">
+        <v>30</v>
+      </c>
+      <c r="M138">
+        <v>0.1</v>
+      </c>
+      <c r="N138">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O138">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="P138">
+        <v>1882.5215161211429</v>
+      </c>
+      <c r="Q138">
+        <v>2</v>
+      </c>
+      <c r="V138">
+        <v>2.1</v>
+      </c>
+      <c r="W138">
+        <v>0.15</v>
+      </c>
+      <c r="X138">
+        <v>500.55024892716472</v>
+      </c>
+      <c r="Z138">
+        <v>982.96093400037421</v>
+      </c>
+      <c r="AF138">
+        <v>1919.2492</v>
+      </c>
+    </row>
+    <row r="139" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>193</v>
+      </c>
+      <c r="C139" t="s">
+        <v>186</v>
+      </c>
+      <c r="D139" t="s">
+        <v>147</v>
+      </c>
+      <c r="E139">
+        <v>8</v>
+      </c>
+      <c r="G139">
+        <v>187</v>
+      </c>
+      <c r="J139">
+        <v>25.2</v>
+      </c>
+      <c r="K139">
+        <v>177.2</v>
+      </c>
+      <c r="L139">
+        <v>30</v>
+      </c>
+      <c r="M139">
+        <v>0.1</v>
+      </c>
+      <c r="N139">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O139">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="P139">
+        <v>925.53143456426778</v>
+      </c>
+      <c r="Q139">
+        <v>30</v>
+      </c>
+      <c r="V139">
+        <v>2.1</v>
+      </c>
+      <c r="W139">
+        <v>0.15</v>
+      </c>
+      <c r="X139">
+        <v>500.7261398392983</v>
+      </c>
+      <c r="Z139">
+        <v>984.36008409501812</v>
+      </c>
+      <c r="AF139">
+        <v>943.58839999999998</v>
+      </c>
+    </row>
+    <row r="140" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>194</v>
+      </c>
+      <c r="C140" t="s">
+        <v>186</v>
+      </c>
+      <c r="D140" t="s">
+        <v>147</v>
+      </c>
+      <c r="E140">
+        <v>9</v>
+      </c>
+      <c r="G140">
+        <v>190</v>
+      </c>
+      <c r="J140">
+        <v>25.2</v>
+      </c>
+      <c r="K140">
+        <v>177</v>
+      </c>
+      <c r="L140">
+        <v>30</v>
+      </c>
+      <c r="M140">
+        <v>0.1</v>
+      </c>
+      <c r="N140">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O140">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="P140">
+        <v>911.74785002230612</v>
+      </c>
+      <c r="Q140">
+        <v>30</v>
+      </c>
+      <c r="V140">
+        <v>2.1</v>
+      </c>
+      <c r="W140">
+        <v>0.15</v>
+      </c>
+      <c r="X140">
+        <v>500.80974090115302</v>
+      </c>
+      <c r="Z140">
+        <v>986.01687134694134</v>
+      </c>
+      <c r="AF140">
+        <v>929.53589999999997</v>
+      </c>
+    </row>
+    <row r="141" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>195</v>
+      </c>
+      <c r="C141" t="s">
+        <v>186</v>
+      </c>
+      <c r="D141" t="s">
+        <v>147</v>
+      </c>
+      <c r="E141">
+        <v>10</v>
+      </c>
+      <c r="G141">
+        <v>191</v>
+      </c>
+      <c r="J141">
+        <v>25.1</v>
+      </c>
+      <c r="K141">
+        <v>176.8</v>
+      </c>
+      <c r="L141">
+        <v>30</v>
+      </c>
+      <c r="M141">
+        <v>0.1</v>
+      </c>
+      <c r="N141">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O141">
+        <v>2263.699354697188</v>
+      </c>
+      <c r="P141">
+        <v>1721.3885991418081</v>
+      </c>
+      <c r="Q141">
+        <v>5</v>
+      </c>
+      <c r="V141">
+        <v>2.1</v>
+      </c>
+      <c r="W141">
+        <v>0.15</v>
+      </c>
+      <c r="X141">
+        <v>500.2175481479556</v>
+      </c>
+      <c r="Z141">
+        <v>982.70424120226198</v>
+      </c>
+      <c r="AF141">
+        <v>1755.0239999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>196</v>
+      </c>
+      <c r="C142" t="s">
+        <v>186</v>
+      </c>
+      <c r="D142" t="s">
+        <v>147</v>
+      </c>
+      <c r="E142">
+        <v>11</v>
+      </c>
+      <c r="J142">
+        <v>25.2</v>
+      </c>
+      <c r="K142">
+        <v>177.15</v>
+      </c>
+      <c r="L142">
+        <v>30</v>
+      </c>
+      <c r="M142">
+        <v>0.1</v>
+      </c>
+      <c r="N142">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O142">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="V142">
+        <v>2.1</v>
+      </c>
+      <c r="W142">
+        <v>0.15</v>
+      </c>
+      <c r="X142">
+        <v>500.79482180302568</v>
+      </c>
+      <c r="Z142">
+        <v>985.106314317017</v>
+      </c>
+    </row>
+    <row r="143" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>197</v>
+      </c>
+      <c r="C143" t="s">
+        <v>186</v>
+      </c>
+      <c r="D143" t="s">
+        <v>147</v>
+      </c>
+      <c r="E143">
+        <v>12</v>
+      </c>
+      <c r="G143">
+        <v>193</v>
+      </c>
+      <c r="J143">
+        <v>25.2</v>
+      </c>
+      <c r="K143">
+        <v>176.95</v>
+      </c>
+      <c r="L143">
+        <v>30</v>
+      </c>
+      <c r="M143">
+        <v>0.1</v>
+      </c>
+      <c r="N143">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O143">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="P143">
+        <v>1503.981371820101</v>
+      </c>
+      <c r="Q143">
+        <v>10</v>
+      </c>
+      <c r="V143">
+        <v>2.1</v>
+      </c>
+      <c r="W143">
+        <v>0.15</v>
+      </c>
+      <c r="X143">
+        <v>500.51038723866111</v>
+      </c>
+      <c r="Z143">
+        <v>983.24735600993574</v>
+      </c>
+      <c r="AF143">
+        <v>1533.3237999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>198</v>
+      </c>
+      <c r="C144" t="s">
+        <v>186</v>
+      </c>
+      <c r="D144" t="s">
+        <v>147</v>
+      </c>
+      <c r="E144">
+        <v>13</v>
+      </c>
+      <c r="G144">
+        <v>195</v>
+      </c>
+      <c r="J144">
+        <v>25.2</v>
+      </c>
+      <c r="K144">
+        <v>176.75</v>
+      </c>
+      <c r="L144">
+        <v>30</v>
+      </c>
+      <c r="M144">
+        <v>0.1</v>
+      </c>
+      <c r="N144">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O144">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="P144">
+        <v>377.26306000475017</v>
+      </c>
+      <c r="Q144">
+        <v>79</v>
+      </c>
+      <c r="V144">
+        <v>2.1</v>
+      </c>
+      <c r="W144">
+        <v>0.15</v>
+      </c>
+      <c r="X144">
+        <v>500.45234459652909</v>
+      </c>
+      <c r="Z144">
+        <v>983.05881868558151</v>
+      </c>
+      <c r="AF144">
+        <v>384.6234</v>
+      </c>
+    </row>
+    <row r="145" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>199</v>
+      </c>
+      <c r="C145" t="s">
+        <v>186</v>
+      </c>
+      <c r="D145" t="s">
+        <v>147</v>
+      </c>
+      <c r="E145">
+        <v>14</v>
+      </c>
+      <c r="G145">
+        <v>196</v>
+      </c>
+      <c r="J145">
+        <v>25.2</v>
+      </c>
+      <c r="K145">
+        <v>176.55</v>
+      </c>
+      <c r="L145">
+        <v>30</v>
+      </c>
+      <c r="M145">
+        <v>0.1</v>
+      </c>
+      <c r="N145">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O145">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="P145">
+        <v>1708.438055684177</v>
+      </c>
+      <c r="Q145">
+        <v>5</v>
+      </c>
+      <c r="V145">
+        <v>2.1</v>
+      </c>
+      <c r="W145">
+        <v>0.15</v>
+      </c>
+      <c r="X145">
+        <v>499.84272738336091</v>
+      </c>
+      <c r="Z145">
+        <v>979.85753478911897</v>
+      </c>
+      <c r="AF145">
+        <v>1741.7693999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>200</v>
+      </c>
+      <c r="C146" t="s">
+        <v>186</v>
+      </c>
+      <c r="D146" t="s">
+        <v>147</v>
+      </c>
+      <c r="E146">
+        <v>15</v>
+      </c>
+      <c r="J146">
+        <v>25.2</v>
+      </c>
+      <c r="K146">
+        <v>177.15</v>
+      </c>
+      <c r="L146">
+        <v>30</v>
+      </c>
+      <c r="M146">
+        <v>0.1</v>
+      </c>
+      <c r="N146">
+        <v>2307.9313400000001</v>
+      </c>
+      <c r="O146">
+        <v>2263.7656461080201</v>
+      </c>
+      <c r="V146">
+        <v>4.2</v>
+      </c>
+      <c r="W146">
+        <v>0.15</v>
+      </c>
+      <c r="X146">
+        <v>632.84611027076664</v>
+      </c>
+      <c r="Z146">
+        <v>2328.747203034643</v>
+      </c>
+    </row>
+    <row r="147" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>201</v>
+      </c>
+      <c r="C147" t="s">
+        <v>202</v>
+      </c>
+      <c r="D147" t="s">
+        <v>34</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <v>1</v>
+      </c>
+      <c r="G147">
+        <v>198</v>
+      </c>
+      <c r="J147">
+        <v>24.8</v>
+      </c>
+      <c r="K147">
+        <v>166.9</v>
+      </c>
+      <c r="L147">
+        <v>30</v>
+      </c>
+      <c r="M147">
+        <v>0.1</v>
+      </c>
+      <c r="N147">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O147">
+        <v>2247.4488218484271</v>
+      </c>
+      <c r="P147">
+        <v>1657.47881326588</v>
+      </c>
+      <c r="Q147">
+        <v>0</v>
+      </c>
+      <c r="R147">
+        <v>625</v>
+      </c>
+      <c r="V147">
+        <v>4.2</v>
+      </c>
+      <c r="W147">
+        <v>0.15</v>
+      </c>
+      <c r="X147">
+        <v>633.20503092788692</v>
+      </c>
+      <c r="Z147">
+        <v>2365.0107161387109</v>
+      </c>
+      <c r="AF147">
+        <v>1690.0130999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>203</v>
+      </c>
+      <c r="C148" t="s">
+        <v>202</v>
+      </c>
+      <c r="D148" t="s">
+        <v>147</v>
+      </c>
+      <c r="E148">
+        <v>2</v>
+      </c>
+      <c r="F148">
+        <v>1</v>
+      </c>
+      <c r="G148">
+        <v>199</v>
+      </c>
+      <c r="J148">
+        <v>25</v>
+      </c>
+      <c r="K148">
+        <v>177.35</v>
+      </c>
+      <c r="L148">
+        <v>30</v>
+      </c>
+      <c r="M148">
+        <v>0.1</v>
+      </c>
+      <c r="N148">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O148">
+        <v>2247.57956598193</v>
+      </c>
+      <c r="P148">
+        <v>1688.8106753165389</v>
+      </c>
+      <c r="Q148">
+        <v>8.3330000000000001E-2</v>
+      </c>
+      <c r="R148">
+        <v>599</v>
+      </c>
+      <c r="V148">
+        <v>4.2</v>
+      </c>
+      <c r="W148">
+        <v>0.15</v>
+      </c>
+      <c r="X148">
+        <v>633.45747696612329</v>
+      </c>
+      <c r="Z148">
+        <v>2326.9495634776731</v>
+      </c>
+      <c r="AF148">
+        <v>1721.8598</v>
+      </c>
+    </row>
+    <row r="149" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>204</v>
+      </c>
+      <c r="C149" t="s">
+        <v>202</v>
+      </c>
+      <c r="D149" t="s">
+        <v>147</v>
+      </c>
+      <c r="E149">
+        <v>3</v>
+      </c>
+      <c r="F149">
+        <v>1</v>
+      </c>
+      <c r="G149">
+        <v>200</v>
+      </c>
+      <c r="J149">
+        <v>25</v>
+      </c>
+      <c r="K149">
+        <v>177.65</v>
+      </c>
+      <c r="L149">
+        <v>30</v>
+      </c>
+      <c r="M149">
+        <v>0.1</v>
+      </c>
+      <c r="N149">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O149">
+        <v>2247.57956598193</v>
+      </c>
+      <c r="P149">
+        <v>1795.9627660196591</v>
+      </c>
+      <c r="Q149">
+        <v>0</v>
+      </c>
+      <c r="V149">
+        <v>3.6</v>
+      </c>
+      <c r="W149">
+        <v>0.15</v>
+      </c>
+      <c r="X149">
+        <v>634.00787348895449</v>
+      </c>
+      <c r="Z149">
+        <v>2330.7948183077378</v>
+      </c>
+      <c r="AF149">
+        <v>1831.1088</v>
+      </c>
+    </row>
+    <row r="150" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>205</v>
+      </c>
+      <c r="C150" t="s">
+        <v>202</v>
+      </c>
+      <c r="D150" t="s">
+        <v>147</v>
+      </c>
+      <c r="E150">
+        <v>4</v>
+      </c>
+      <c r="F150">
+        <v>1</v>
+      </c>
+      <c r="G150">
+        <v>201</v>
+      </c>
+      <c r="J150">
+        <v>25.1</v>
+      </c>
+      <c r="K150">
+        <v>177.95</v>
+      </c>
+      <c r="L150">
+        <v>30</v>
+      </c>
+      <c r="M150">
+        <v>0.1</v>
+      </c>
+      <c r="N150">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O150">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P150">
+        <v>1847.5906500963131</v>
+      </c>
+      <c r="Q150">
+        <v>0</v>
+      </c>
+      <c r="V150">
+        <v>3</v>
+      </c>
+      <c r="W150">
+        <v>0.15</v>
+      </c>
+      <c r="X150">
+        <v>634.45775278600865</v>
+      </c>
+      <c r="Z150">
+        <v>2328.7730451283269</v>
+      </c>
+      <c r="AF150">
+        <v>1883.692</v>
+      </c>
+    </row>
+    <row r="151" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>206</v>
+      </c>
+      <c r="C151" t="s">
+        <v>202</v>
+      </c>
+      <c r="D151" t="s">
+        <v>147</v>
+      </c>
+      <c r="E151">
+        <v>5</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
+      </c>
+      <c r="G151">
+        <v>202</v>
+      </c>
+      <c r="J151">
+        <v>25.1</v>
+      </c>
+      <c r="K151">
+        <v>177.7</v>
+      </c>
+      <c r="L151">
+        <v>30</v>
+      </c>
+      <c r="M151">
+        <v>0.1</v>
+      </c>
+      <c r="N151">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O151">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P151">
+        <v>1923.4982392794029</v>
+      </c>
+      <c r="Q151">
+        <v>8.3333000000000004E-2</v>
+      </c>
+      <c r="V151">
+        <v>2.4</v>
+      </c>
+      <c r="W151">
+        <v>0.15</v>
+      </c>
+      <c r="AF151">
+        <v>1961.0827999999999</v>
+      </c>
+    </row>
+    <row r="152" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
+        <v>207</v>
+      </c>
+      <c r="C152" t="s">
+        <v>202</v>
+      </c>
+      <c r="D152" t="s">
+        <v>147</v>
+      </c>
+      <c r="E152">
+        <v>6</v>
+      </c>
+      <c r="F152">
+        <v>1</v>
+      </c>
+      <c r="G152">
+        <v>203</v>
+      </c>
+      <c r="J152">
+        <v>25.2</v>
+      </c>
+      <c r="K152">
+        <v>177.75</v>
+      </c>
+      <c r="L152">
+        <v>30</v>
+      </c>
+      <c r="M152">
+        <v>0.1</v>
+      </c>
+      <c r="N152">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O152">
+        <v>2247.7110290356632</v>
+      </c>
+      <c r="P152">
+        <v>1990.07555459323</v>
+      </c>
+      <c r="Q152">
+        <v>0</v>
+      </c>
+      <c r="V152">
+        <v>2.1</v>
+      </c>
+      <c r="W152">
+        <v>0.15</v>
+      </c>
+      <c r="X152">
+        <v>501.76745350947863</v>
+      </c>
+      <c r="Z152">
+        <v>983.11498351008049</v>
+      </c>
+      <c r="AF152">
+        <v>2028.9015999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>208</v>
+      </c>
+      <c r="C153" t="s">
+        <v>202</v>
+      </c>
+      <c r="D153" t="s">
+        <v>147</v>
+      </c>
+      <c r="E153">
+        <v>7</v>
+      </c>
+      <c r="F153">
+        <v>1</v>
+      </c>
+      <c r="G153">
+        <v>204</v>
+      </c>
+      <c r="J153">
+        <v>25.1</v>
+      </c>
+      <c r="K153">
+        <v>177.5</v>
+      </c>
+      <c r="L153">
+        <v>30</v>
+      </c>
+      <c r="M153">
+        <v>0.1</v>
+      </c>
+      <c r="N153">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O153">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P153">
+        <v>2046.183997506331</v>
+      </c>
+      <c r="Q153">
+        <v>0</v>
+      </c>
+      <c r="R153">
+        <v>292</v>
+      </c>
+      <c r="V153">
+        <v>1.8</v>
+      </c>
+      <c r="W153">
+        <v>0.15</v>
+      </c>
+      <c r="X153">
+        <v>473.93480487280817</v>
+      </c>
+      <c r="Z153">
+        <v>453.56917604809689</v>
+      </c>
+      <c r="AF153">
+        <v>2086.1658000000002</v>
+      </c>
+    </row>
+    <row r="154" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
+        <v>209</v>
+      </c>
+      <c r="C154" t="s">
+        <v>202</v>
+      </c>
+      <c r="D154" t="s">
+        <v>147</v>
+      </c>
+      <c r="E154">
+        <v>8</v>
+      </c>
+      <c r="F154">
+        <v>1</v>
+      </c>
+      <c r="G154">
+        <v>205</v>
+      </c>
+      <c r="J154">
+        <v>25.1</v>
+      </c>
+      <c r="K154">
+        <v>177.3</v>
+      </c>
+      <c r="L154">
+        <v>30</v>
+      </c>
+      <c r="M154">
+        <v>0.1</v>
+      </c>
+      <c r="N154">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O154">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P154">
+        <v>2074.647136571708</v>
+      </c>
+      <c r="Q154">
+        <v>0.16666600000000001</v>
+      </c>
+      <c r="R154">
+        <v>270</v>
+      </c>
+      <c r="V154">
+        <v>1.5</v>
+      </c>
+      <c r="W154">
+        <v>0.15</v>
+      </c>
+      <c r="X154">
+        <v>469.4633541918829</v>
+      </c>
+      <c r="Z154">
+        <v>386.19905496188608</v>
+      </c>
+      <c r="AF154">
+        <v>2115.1851000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
+        <v>210</v>
+      </c>
+      <c r="C155" t="s">
+        <v>202</v>
+      </c>
+      <c r="D155" t="s">
+        <v>147</v>
+      </c>
+      <c r="E155">
+        <v>9</v>
+      </c>
+      <c r="F155">
+        <v>1</v>
+      </c>
+      <c r="G155">
+        <v>206</v>
+      </c>
+      <c r="J155">
+        <v>25.1</v>
+      </c>
+      <c r="K155">
+        <v>177.15</v>
+      </c>
+      <c r="L155">
+        <v>30</v>
+      </c>
+      <c r="M155">
+        <v>0.1</v>
+      </c>
+      <c r="N155">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O155">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P155">
+        <v>2088.176085101496</v>
+      </c>
+      <c r="Q155">
+        <v>1.166666</v>
+      </c>
+      <c r="R155">
+        <v>219</v>
+      </c>
+      <c r="V155">
+        <v>1.2</v>
+      </c>
+      <c r="W155">
+        <v>0.15</v>
+      </c>
+      <c r="X155">
+        <v>460.53497175822503</v>
+      </c>
+      <c r="Z155">
+        <v>233.1054578909156</v>
+      </c>
+      <c r="AF155">
+        <v>2128.9784</v>
+      </c>
+    </row>
+    <row r="156" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B156" t="s">
+        <v>211</v>
+      </c>
+      <c r="C156" t="s">
+        <v>202</v>
+      </c>
+      <c r="D156" t="s">
+        <v>147</v>
+      </c>
+      <c r="E156">
+        <v>10</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+      <c r="G156">
+        <v>207</v>
+      </c>
+      <c r="J156">
+        <v>25.1</v>
+      </c>
+      <c r="K156">
+        <v>177.1</v>
+      </c>
+      <c r="L156">
+        <v>30</v>
+      </c>
+      <c r="M156">
+        <v>0.1</v>
+      </c>
+      <c r="N156">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O156">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P156">
+        <v>2110.2330978930599</v>
+      </c>
+      <c r="Q156">
+        <v>0</v>
+      </c>
+      <c r="R156">
+        <v>219</v>
+      </c>
+      <c r="V156">
+        <v>1.2</v>
+      </c>
+      <c r="W156">
+        <v>0.15</v>
+      </c>
+      <c r="X156">
+        <v>460.28603855912212</v>
+      </c>
+      <c r="Z156">
+        <v>232.18811934360519</v>
+      </c>
+      <c r="AF156">
+        <v>2151.4663999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B157" t="s">
+        <v>212</v>
+      </c>
+      <c r="C157" t="s">
+        <v>202</v>
+      </c>
+      <c r="D157" t="s">
+        <v>147</v>
+      </c>
+      <c r="E157">
+        <v>11</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+      <c r="G157">
+        <v>208</v>
+      </c>
+      <c r="J157">
+        <v>25.1</v>
+      </c>
+      <c r="K157">
+        <v>175.6</v>
+      </c>
+      <c r="L157">
+        <v>30</v>
+      </c>
+      <c r="M157">
+        <v>0.1</v>
+      </c>
+      <c r="N157">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O157">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P157">
+        <v>2181.8628742164419</v>
+      </c>
+      <c r="Q157">
+        <v>0</v>
+      </c>
+      <c r="R157">
+        <v>114</v>
+      </c>
+      <c r="V157">
+        <v>0.6</v>
+      </c>
+      <c r="W157">
+        <v>0.15</v>
+      </c>
+      <c r="X157">
+        <v>450.01328287875742</v>
+      </c>
+      <c r="Z157">
+        <v>120.93377186325451</v>
+      </c>
+      <c r="AF157">
+        <v>2224.4958000000001</v>
+      </c>
+    </row>
+    <row r="158" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>213</v>
+      </c>
+      <c r="C158" t="s">
+        <v>202</v>
+      </c>
+      <c r="D158" t="s">
+        <v>147</v>
+      </c>
+      <c r="E158">
+        <v>12</v>
+      </c>
+      <c r="F158">
+        <v>1</v>
+      </c>
+      <c r="G158">
+        <v>209</v>
+      </c>
+      <c r="J158">
+        <v>25.1</v>
+      </c>
+      <c r="L158">
+        <v>30</v>
+      </c>
+      <c r="M158">
+        <v>0.1</v>
+      </c>
+      <c r="N158">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O158">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P158">
+        <v>2236.5688366296481</v>
+      </c>
+      <c r="Q158">
+        <v>0</v>
+      </c>
+      <c r="R158">
+        <v>0</v>
+      </c>
+      <c r="V158">
+        <v>0.15</v>
+      </c>
+      <c r="W158">
+        <v>0.15</v>
+      </c>
+      <c r="AF158">
+        <v>2280.2707</v>
+      </c>
+    </row>
+    <row r="159" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B159" t="s">
+        <v>214</v>
+      </c>
+      <c r="C159" t="s">
+        <v>202</v>
+      </c>
+      <c r="D159" t="s">
+        <v>147</v>
+      </c>
+      <c r="E159">
+        <v>13</v>
+      </c>
+      <c r="F159">
+        <v>2</v>
+      </c>
+      <c r="G159">
+        <v>211</v>
+      </c>
+      <c r="J159">
+        <v>25.1</v>
+      </c>
+      <c r="L159">
+        <v>30</v>
+      </c>
+      <c r="M159">
+        <v>0.1</v>
+      </c>
+      <c r="N159">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O159">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P159">
+        <v>2225.4638251201281</v>
+      </c>
+      <c r="Q159">
+        <v>0</v>
+      </c>
+      <c r="R159">
+        <v>0</v>
+      </c>
+      <c r="V159">
+        <v>0</v>
+      </c>
+      <c r="W159">
+        <v>0.15</v>
+      </c>
+      <c r="AF159">
+        <v>2268.9486999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B160" t="s">
+        <v>215</v>
+      </c>
+      <c r="C160" t="s">
+        <v>202</v>
+      </c>
+      <c r="D160" t="s">
+        <v>147</v>
+      </c>
+      <c r="E160">
+        <v>14</v>
+      </c>
+      <c r="F160">
+        <v>2</v>
+      </c>
+      <c r="G160">
+        <v>213</v>
+      </c>
+      <c r="J160">
+        <v>25.1</v>
+      </c>
+      <c r="L160">
+        <v>30</v>
+      </c>
+      <c r="M160">
+        <v>0.1</v>
+      </c>
+      <c r="N160">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O160">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P160">
+        <v>2100.823263153713</v>
+      </c>
+      <c r="Q160">
+        <v>86</v>
+      </c>
+      <c r="R160">
+        <v>0</v>
+      </c>
+      <c r="V160">
+        <v>0.15</v>
+      </c>
+      <c r="W160">
+        <v>0.15</v>
+      </c>
+      <c r="AF160">
+        <v>2141.8726999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B161" t="s">
+        <v>216</v>
+      </c>
+      <c r="C161" t="s">
+        <v>202</v>
+      </c>
+      <c r="D161" t="s">
+        <v>147</v>
+      </c>
+      <c r="E161">
+        <v>15</v>
+      </c>
+      <c r="F161">
+        <v>2</v>
+      </c>
+      <c r="G161">
+        <v>214</v>
+      </c>
+      <c r="J161">
+        <v>25.1</v>
+      </c>
+      <c r="L161">
+        <v>30</v>
+      </c>
+      <c r="M161">
+        <v>0.1</v>
+      </c>
+      <c r="N161">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O161">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P161">
+        <v>2232.4895447317422</v>
+      </c>
+      <c r="Q161">
+        <v>0</v>
+      </c>
+      <c r="R161">
+        <v>0</v>
+      </c>
+      <c r="V161">
+        <v>0.15</v>
+      </c>
+      <c r="W161">
+        <v>0.15</v>
+      </c>
+      <c r="AF161">
+        <v>2276.1116999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B162" t="s">
+        <v>217</v>
+      </c>
+      <c r="C162" t="s">
+        <v>202</v>
+      </c>
+      <c r="D162" t="s">
+        <v>147</v>
+      </c>
+      <c r="E162">
+        <v>16</v>
+      </c>
+      <c r="F162">
+        <v>2</v>
+      </c>
+      <c r="G162">
+        <v>215</v>
+      </c>
+      <c r="J162">
+        <v>25.1</v>
+      </c>
+      <c r="L162">
+        <v>30</v>
+      </c>
+      <c r="M162">
+        <v>0.1</v>
+      </c>
+      <c r="N162">
+        <v>2291.5635000000002</v>
+      </c>
+      <c r="O162">
+        <v>2247.6452077632562</v>
+      </c>
+      <c r="P162">
+        <v>2242.0296343314012</v>
+      </c>
+      <c r="Q162">
+        <v>0</v>
+      </c>
+      <c r="R162">
+        <v>0</v>
+      </c>
+      <c r="V162">
+        <v>0</v>
+      </c>
+      <c r="W162">
+        <v>0.15</v>
+      </c>
+      <c r="AF162">
+        <v>2285.8382000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add and update DIC modeling and analysis scripts
Added new scripts for modeling C-parameter, combining predicted and measured DIC, and analyzing variable DIC effects. Improved DIC decay plotting, updated titration fit analysis, and made minor changes to modify_dic.py. Updated Logbook_automated_by_python_testing.xlsx with new data.
</commit_message>
<xml_diff>
--- a/Logbook_automated_by_python_testing.xlsx
+++ b/Logbook_automated_by_python_testing.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="165" documentId="11_2AF9439815536E0E62355476585DCE3A8741D500" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED1ED462-CC00-473B-A309-9C722672F892}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="31110" yWindow="2370" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2442,7 +2442,7 @@
   <dimension ref="A1:AG339"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>